<commit_message>
learn how to format cells
</commit_message>
<xml_diff>
--- a/monthly-budget.xlsx
+++ b/monthly-budget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MSI\Desktop\Learning Excel\excel-exercises\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCDA68C5-0BF6-459B-AFC5-A884E4A25A4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F8454BF-9EBC-47C7-8C32-C8AB1A232081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{7BDB811D-95D9-48C3-9726-37E9EF4607BC}"/>
   </bookViews>
@@ -90,7 +90,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,16 +110,53 @@
       <charset val="162"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color theme="0"/>
+      <name val="Arial Black"/>
+      <family val="2"/>
+      <charset val="162"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -123,17 +164,53 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="3"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="for-budget" xfId="3" xr:uid="{17670243-3C9C-4F23-98F7-835E9641B2D4}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -443,301 +520,320 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D46F3BD-4151-4600-925F-A8361B6312C9}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="B2:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="7" width="12" customWidth="1"/>
+    <col min="1" max="1" width="8.7265625" customWidth="1"/>
+    <col min="2" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="11.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="2" spans="2:8" ht="37.5" thickBot="1" x14ac:dyDescent="1.1000000000000001">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+    </row>
+    <row r="4" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H4" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="C5" s="1">
         <v>300</v>
       </c>
-      <c r="C4">
+      <c r="D5" s="1">
         <v>350</v>
       </c>
-      <c r="D4">
+      <c r="E5" s="1">
         <v>325</v>
       </c>
-      <c r="E4">
+      <c r="F5" s="1">
         <v>310</v>
       </c>
-      <c r="F4">
-        <f>SUM(B4:E4)</f>
+      <c r="G5" s="1">
+        <f>SUM(C5:F5)</f>
         <v>1285</v>
       </c>
-      <c r="G4">
-        <f>F4/$F$9</f>
+      <c r="H5" s="3">
+        <f>G5/$G$10</f>
         <v>0.19528875379939209</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
         <v>16</v>
       </c>
-      <c r="B5">
+      <c r="C6" s="2">
         <v>50</v>
       </c>
-      <c r="C5">
+      <c r="D6" s="2">
         <v>50</v>
       </c>
-      <c r="D5">
+      <c r="E6" s="2">
         <v>50</v>
       </c>
-      <c r="E5">
+      <c r="F6" s="2">
         <v>50</v>
       </c>
-      <c r="F5">
-        <f>SUM(B5:E5)</f>
+      <c r="G6" s="2">
+        <f>SUM(C6:F6)</f>
         <v>200</v>
       </c>
-      <c r="G5">
-        <f>F5/$F$9</f>
+      <c r="H6" s="3">
+        <f>G6/$G$10</f>
         <v>3.0395136778115502E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
         <v>3</v>
       </c>
-      <c r="B6">
+      <c r="C7" s="2">
         <v>150</v>
       </c>
-      <c r="C6">
+      <c r="D7" s="2">
         <v>175</v>
       </c>
-      <c r="D6">
+      <c r="E7" s="2">
         <v>175</v>
       </c>
-      <c r="E6">
+      <c r="F7" s="2">
         <v>210</v>
       </c>
-      <c r="F6">
-        <f>SUM(B6:E6)</f>
+      <c r="G7" s="2">
+        <f>SUM(C7:F7)</f>
         <v>710</v>
       </c>
-      <c r="G6">
-        <f>F6/$F$9</f>
+      <c r="H7" s="3">
+        <f>G7/$G$10</f>
         <v>0.10790273556231003</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
         <v>4</v>
       </c>
-      <c r="B7">
+      <c r="C8" s="2">
         <v>100</v>
       </c>
-      <c r="C7">
+      <c r="D8" s="2">
         <v>110</v>
       </c>
-      <c r="D7">
+      <c r="E8" s="2">
         <v>80</v>
       </c>
-      <c r="E7">
+      <c r="F8" s="2">
         <v>95</v>
       </c>
-      <c r="F7">
-        <f>SUM(B7:E7)</f>
+      <c r="G8" s="2">
+        <f>SUM(C8:F8)</f>
         <v>385</v>
       </c>
-      <c r="G7">
-        <f>F7/$F$9</f>
+      <c r="H8" s="3">
+        <f>G8/$G$10</f>
         <v>5.8510638297872342E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
         <v>6</v>
       </c>
-      <c r="B8">
+      <c r="C9" s="2">
         <v>1000</v>
       </c>
-      <c r="C8">
+      <c r="D9" s="2">
         <v>1000</v>
       </c>
-      <c r="D8">
+      <c r="E9" s="2">
         <v>1000</v>
       </c>
-      <c r="E8">
+      <c r="F9" s="2">
         <v>1000</v>
       </c>
-      <c r="F8">
-        <f>SUM(B8:E8)</f>
+      <c r="G9" s="2">
+        <f>SUM(C9:F9)</f>
         <v>4000</v>
       </c>
-      <c r="G8">
-        <f>F8/$F$9</f>
+      <c r="H9" s="3">
+        <f>G9/$G$10</f>
         <v>0.60790273556231</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
         <v>5</v>
       </c>
-      <c r="B9">
-        <f t="shared" ref="B9:E9" si="0">SUM(B4:B8)</f>
+      <c r="C10" s="1">
+        <f t="shared" ref="C10:F10" si="0">SUM(C5:C9)</f>
         <v>1600</v>
       </c>
-      <c r="C9">
+      <c r="D10" s="1">
         <f t="shared" si="0"/>
         <v>1685</v>
       </c>
-      <c r="D9">
+      <c r="E10" s="1">
         <f t="shared" si="0"/>
         <v>1630</v>
       </c>
-      <c r="E9">
+      <c r="F10" s="1">
         <f t="shared" si="0"/>
         <v>1665</v>
       </c>
-      <c r="F9">
-        <f>SUM(F4:F8)</f>
+      <c r="G10" s="1">
+        <f>SUM(G5:G9)</f>
         <v>6580</v>
       </c>
-      <c r="G9">
-        <f>F9/$F$9</f>
+      <c r="H10" s="3">
+        <f>G10/$G$10</f>
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="2:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B11">
-        <f>MIN(B4:B8)</f>
+      <c r="C12">
+        <f>MIN(C5:C9)</f>
         <v>50</v>
       </c>
-      <c r="C11">
-        <f t="shared" ref="C11:F11" si="1">MIN(C4:C8)</f>
+      <c r="D12">
+        <f t="shared" ref="D12:G12" si="1">MIN(D5:D9)</f>
         <v>50</v>
       </c>
-      <c r="D11">
+      <c r="E12">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="E11">
+      <c r="F12">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="F11">
+      <c r="G12">
         <f t="shared" si="1"/>
         <v>200</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+    <row r="13" spans="2:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B12">
-        <f>MAX(B4:B8)</f>
+      <c r="C13">
+        <f>MAX(C5:C9)</f>
         <v>1000</v>
       </c>
-      <c r="C12">
-        <f t="shared" ref="C12:F12" si="2">MAX(C4:C8)</f>
+      <c r="D13">
+        <f t="shared" ref="D13:G13" si="2">MAX(D5:D9)</f>
         <v>1000</v>
       </c>
-      <c r="D12">
+      <c r="E13">
         <f t="shared" si="2"/>
         <v>1000</v>
       </c>
-      <c r="E12">
+      <c r="F13">
         <f t="shared" si="2"/>
         <v>1000</v>
       </c>
-      <c r="F12">
+      <c r="G13">
         <f t="shared" si="2"/>
         <v>4000</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+    <row r="14" spans="2:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B13">
-        <f>AVERAGE(B4:B8)</f>
+      <c r="C14">
+        <f>AVERAGE(C5:C9)</f>
         <v>320</v>
       </c>
-      <c r="C13">
-        <f t="shared" ref="C13:F13" si="3">AVERAGE(C4:C8)</f>
+      <c r="D14">
+        <f t="shared" ref="D14:G14" si="3">AVERAGE(D5:D9)</f>
         <v>337</v>
       </c>
-      <c r="D13">
+      <c r="E14">
         <f t="shared" si="3"/>
         <v>326</v>
       </c>
-      <c r="E13">
+      <c r="F14">
         <f t="shared" si="3"/>
         <v>333</v>
       </c>
-      <c r="F13">
+      <c r="G14">
         <f t="shared" si="3"/>
         <v>1316</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+    <row r="15" spans="2:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B15" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B14">
-        <f>COUNT(B4:B8)</f>
+      <c r="C15">
+        <f>COUNT(C5:C9)</f>
         <v>5</v>
       </c>
-      <c r="C14">
-        <f t="shared" ref="C14:F14" si="4">COUNT(C4:C8)</f>
+      <c r="D15">
+        <f t="shared" ref="D15:G15" si="4">COUNT(D5:D9)</f>
         <v>5</v>
       </c>
-      <c r="D14">
+      <c r="E15">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="E14">
+      <c r="F15">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="F14">
+      <c r="G15">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:H2"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="C5:F9">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>200</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>